<commit_message>
Warn if Min desired scholarship cannot be met
</commit_message>
<xml_diff>
--- a/Scholarship Forcasting Calculator.xlsx
+++ b/Scholarship Forcasting Calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pooteron\dev\jonmat\ScholarshipTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47839ACF-F6CE-4950-B991-397FC281D368}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1E9098-8246-4807-80FD-5E8036925AA2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A691991B-D22E-4950-8C31-DEB8144FF473}"/>
   </bookViews>
@@ -684,7 +684,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C12" t="str">
-        <f>IF(AND(I12&gt;= 0, I13&lt;0), "Last Year====&gt;", IF(AND(SUM(L12:L37)-SUM(E12:E37)&gt;= 0, SUM(L13:L38)-SUM(E13:E38)&lt;0), "25 Year Warn====&gt;", ""))</f>
+        <f>IF(AND(I12&gt;= 0, I13&lt;0), "Last Year====&gt;", IF(SUM(L13:L38)-SUM(E13:E38)&lt;0, "!!!Min Scholarship Not Met!!!", ""))</f>
         <v/>
       </c>
       <c r="D12">
@@ -754,7 +754,7 @@
         <v>2</v>
       </c>
       <c r="L13" s="1">
-        <f t="shared" ref="L12:L75" si="5">MIN( (G13*(Scholarship/100))-MOD((G13*(Scholarship/100)), NearestRound),MAX(0,(I13*(InvestReturn-K13)/100)-MOD((I13*(InvestReturn-K13)/100), NearestRound)))</f>
+        <f t="shared" ref="L13:L75" si="5">MIN( (G13*(Scholarship/100))-MOD((G13*(Scholarship/100)), NearestRound),MAX(0,(I13*(InvestReturn-K13)/100)-MOD((I13*(InvestReturn-K13)/100), NearestRound)))</f>
         <v>3000</v>
       </c>
     </row>
@@ -20172,7 +20172,7 @@
         <v>2</v>
       </c>
       <c r="L524" s="1">
-        <f t="shared" ref="L524:L587" si="51">MIN( (G524*(Scholarship/100))-MOD((G524*(Scholarship/100)), NearestRound),MAX(0,(I524*(InvestReturn-K524)/100)-MOD((I524*(InvestReturn-K524)/100), NearestRound)))</f>
+        <f t="shared" ref="L524:L552" si="51">MIN( (G524*(Scholarship/100))-MOD((G524*(Scholarship/100)), NearestRound),MAX(0,(I524*(InvestReturn-K524)/100)-MOD((I524*(InvestReturn-K524)/100), NearestRound)))</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>